<commit_message>
Update Scenario Analysis Video - Start.xlsx
</commit_message>
<xml_diff>
--- a/Financial Models/Scenario Analysis Video - Start.xlsx
+++ b/Financial Models/Scenario Analysis Video - Start.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markw\OneDrive - Zomalex Ltd\Courses\Course - Excel\Spreadsheet Modelling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markw\Documents\GitHub\lbag-online\Financial Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB576664-9EE7-4E9B-A964-6E398FC86FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DEC2D3-40DB-4318-A183-848DCB950A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="75" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5EBE0B45-FAEE-4C9D-85E7-DA9E952C6525}"/>
   </bookViews>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4A7ABD-E875-458A-A3D5-7CC95DF48CA6}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1403,8 @@
         <v>3</v>
       </c>
       <c r="C47" s="48">
-        <v>0.2</v>
+        <f>B9</f>
+        <v>0.12</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>

</xml_diff>